<commit_message>
Layout salario masivo, cambio en la sabana
</commit_message>
<xml_diff>
--- a/Payroll/Content/FilesUpsSalary/AJUSTES DE SUELDOS IPS (1).xlsx
+++ b/Payroll/Content/FilesUpsSalary/AJUSTES DE SUELDOS IPS (1).xlsx
@@ -488,19 +488,21 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>4</v>
@@ -528,7 +530,7 @@
       <c r="D2" s="6">
         <v>4</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2">
         <v>11102</v>
       </c>
       <c r="F2">
@@ -538,7 +540,7 @@
         <v>5500</v>
       </c>
       <c r="H2" s="5">
-        <v>44348</v>
+        <v>44361</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -549,13 +551,13 @@
         <v>11005</v>
       </c>
       <c r="F3">
-        <v>352</v>
+        <v>643</v>
       </c>
       <c r="G3" s="4">
         <v>14666.666666666668</v>
       </c>
       <c r="H3" s="5">
-        <v>44348</v>
+        <v>44361</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -572,7 +574,7 @@
         <v>9666.6666666666679</v>
       </c>
       <c r="H4" s="5">
-        <v>44348</v>
+        <v>44360</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -583,13 +585,13 @@
         <v>21430</v>
       </c>
       <c r="F5">
-        <v>352</v>
+        <v>3323</v>
       </c>
       <c r="G5" s="4">
         <v>9666.6666666666679</v>
       </c>
       <c r="H5" s="5">
-        <v>44348</v>
+        <v>44359</v>
       </c>
     </row>
   </sheetData>

</xml_diff>